<commit_message>
Added CEview() method to MainWin
Changed the types for the buffs and MLBBuffs fields of the CE.class to String. From the way CEs are set up, it's likely easier/better for a user to input Strings to describe the effects. Will likely use a multi-dimensional ArrayLists when implementing the Servant class in the future. Updated the UML to reflect the changes in the CEclass. Also updated the setters/getters to handle Strings.

On the MainWin class, added a CEview() method that is called from within the MouseListener. CEview uses a CE paramter, with the CE being retrieved from the database based on which row was clicked from within the JTable. CEview opens up a new JDialog and the CE information is added as seperate JLabels. There are 3 different sets of GridBagConstraints. Currently trying to format the JDialog so that the information is displayed uniformly. This might include changing fonts/sizes, and having the fullPortrait be somewhat scalable.
</commit_message>
<xml_diff>
--- a/FGO_ServantWiki/Scrum.xlsx
+++ b/FGO_ServantWiki/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuroi\Documents\NetBeansProjects\GitPersonal-Projects\FGO_ServantWiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A9D423-84CE-4F7F-8F98-ABA9253F6F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330C2C58-0EC5-4AEB-82FE-DD2E98A99A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34290" yWindow="1530" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{EC6440E6-F9F1-4899-A339-3D59A18A2AAF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
   <si>
     <t>Product Name:</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>Create a viewing area within MainWin to view icons of available CEs within the database</t>
+  </si>
+  <si>
+    <t>Create a JDialog to view CE information from MainWin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete </t>
+  </si>
+  <si>
+    <t>Currently trying to format the Jdialog</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -673,20 +685,20 @@
       <selection activeCell="I10" sqref="I10:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="97.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="97.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -729,7 +741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -746,7 +758,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -760,7 +772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -780,7 +792,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -797,7 +809,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -811,7 +823,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -825,7 +837,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -839,7 +851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -853,7 +865,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -873,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -890,7 +902,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -910,7 +922,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -930,7 +942,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -947,7 +959,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -961,7 +973,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -975,7 +987,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -986,7 +998,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1000,7 +1012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1014,7 +1026,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1039,22 +1051,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED33CBF-243B-4856-813E-0293B3B9E74E}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.26953125" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
-    <col min="6" max="6" width="87.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="87.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1075,7 +1087,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1095,7 +1107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -1109,7 +1121,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>77</v>
       </c>
@@ -1123,7 +1135,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>57</v>
       </c>
@@ -1137,7 +1149,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>61</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>61</v>
       </c>
@@ -1159,59 +1171,73 @@
         <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
         <v>88</v>
       </c>
       <c r="F9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>87</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>85</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CE Implementation Finished (more or less)
Successfully implemented the input window to enter in new CE information to add onto the database.

I'll say that Sprint 1 is more or less finished and will start on Sprint 2 soon. Will be carrying over the ToolBar and About Features from Sprint 1 over. Sprint 2 will deal with the saving and loading information from some file into the database so that the data will persist over time.

After reviewing some of the later CEs, I remembered that some CEs have 2 effects. The 2nd effect is usually something that only comes into play during a limited Event period. Will likely have to think of some way to include this.
</commit_message>
<xml_diff>
--- a/FGO_ServantWiki/Scrum.xlsx
+++ b/FGO_ServantWiki/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuroi\Documents\NetBeansProjects\GitPersonal-Projects\FGO_ServantWiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7654975-7852-49B3-97A0-ED265F732A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2876DD9-F3B7-4489-A9D3-8C5A90AA756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="1530" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{EC6440E6-F9F1-4899-A339-3D59A18A2AAF}"/>
+    <workbookView xWindow="34290" yWindow="1530" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="1" xr2:uid="{EC6440E6-F9F1-4899-A339-3D59A18A2AAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,7 +1210,7 @@
         <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Start of Sprint 2
Updated the UML for this personal project.
</commit_message>
<xml_diff>
--- a/FGO_ServantWiki/Scrum.xlsx
+++ b/FGO_ServantWiki/Scrum.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuroi\Documents\NetBeansProjects\GitPersonal-Projects\FGO_ServantWiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2876DD9-F3B7-4489-A9D3-8C5A90AA756A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE33D3EB-7F29-4FFE-9D16-7F77CA5A60D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="1530" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="1" xr2:uid="{EC6440E6-F9F1-4899-A339-3D59A18A2AAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{EC6440E6-F9F1-4899-A339-3D59A18A2AAF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
   <si>
     <t>Product Name:</t>
   </si>
@@ -324,6 +325,39 @@
   </si>
   <si>
     <t>Functionally it works; Will need to go back and try and format the view window</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Save database data into a separate file</t>
+  </si>
+  <si>
+    <t>Goal is to be able to retain data over the years</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Open and load database data from a separate file</t>
+  </si>
+  <si>
+    <t>The opposite of the Save feature. Allows to load previous database data.</t>
+  </si>
+  <si>
+    <t>These functions are pertaining the CE portion of the database.</t>
+  </si>
+  <si>
+    <t>EventEff</t>
+  </si>
+  <si>
+    <t>Implement some way to add Event specific effects for Ces</t>
+  </si>
+  <si>
+    <t>Add limited time effects for certain Ces</t>
+  </si>
+  <si>
+    <t>Inprogress</t>
   </si>
 </sst>
 </file>
@@ -339,12 +373,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -359,12 +399,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,383 +720,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0A2C5E-1169-4FAC-9CE9-818A6961BC7A}">
-  <dimension ref="A1:K36"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="97.85546875" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="I21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="I22" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="I23" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="I24" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" t="s">
-        <v>42</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="I25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="I26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="I27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34">
-        <v>3</v>
-      </c>
-      <c r="I34" t="s">
-        <v>51</v>
-      </c>
-      <c r="J34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35">
-        <v>3</v>
-      </c>
-      <c r="I35" t="s">
-        <v>52</v>
-      </c>
-      <c r="J35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36">
-        <v>3</v>
-      </c>
-      <c r="I36" t="s">
-        <v>53</v>
-      </c>
-      <c r="J36" t="s">
-        <v>55</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED33CBF-243B-4856-813E-0293B3B9E74E}">
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,4 +921,638 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E591C3-18B1-4F40-8494-0A20B36F04D6}">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" customWidth="1"/>
+    <col min="6" max="6" width="97.28515625" customWidth="1"/>
+    <col min="9" max="9" width="41.28515625" customWidth="1"/>
+    <col min="10" max="10" width="42.42578125" customWidth="1"/>
+    <col min="11" max="11" width="75.28515625" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0A2C5E-1169-4FAC-9CE9-818A6961BC7A}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="53.7109375" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" customWidth="1"/>
+    <col min="11" max="11" width="97.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>